<commit_message>
Adding references to the ERASMUS Project
</commit_message>
<xml_diff>
--- a/References/Literature Review - ERASMUS Project.xlsx
+++ b/References/Literature Review - ERASMUS Project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\axelh\OneDrive\Documents\Hydroinformatics\ERASMUS_Project\References\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{956AB6DB-523C-4D41-979F-580B2C99AA9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9CC26A-B2DD-4FFB-9310-4577EEB88852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{33D79010-2EAD-46DA-9565-688F701BD65C}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="110">
   <si>
     <t>FOR: IRRIGATION SCHEDULING</t>
   </si>
@@ -396,9 +396,6 @@
     <t>Publisher</t>
   </si>
   <si>
-    <t>Agricultural Water Management</t>
-  </si>
-  <si>
     <t>Optimization Tool to Improve the Management of the Leakages and Recovered Energy in Irrigation Water Systems</t>
   </si>
   <si>
@@ -411,7 +408,22 @@
     <t>2021</t>
   </si>
   <si>
-    <t>Water meter reading</t>
+    <t>Leakage Detection in Water Networks by a Calibration Method</t>
+  </si>
+  <si>
+    <t>Elsevier - Flow Measurement and Instrumentation</t>
+  </si>
+  <si>
+    <t>Elsevier - Agricultural Water Management</t>
+  </si>
+  <si>
+    <t>Pressure and flow meter sensors.</t>
+  </si>
+  <si>
+    <t>Flow meter sensors.</t>
+  </si>
+  <si>
+    <t>The zone with the most leakage was identified by analysing the result of pressure sensors. Node demands and pipe roughness were calibrated with a metaheuristic optimization algorithm. Then the probability of leakage in each sub-zone was estimated.</t>
   </si>
 </sst>
 </file>
@@ -1439,8 +1451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7117D393-370F-41E6-8475-B08505AFF5F4}">
   <dimension ref="B2:I19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1485,7 +1497,7 @@
         <v>3</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H5" s="12" t="s">
         <v>5</v>
@@ -1499,32 +1511,42 @@
         <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>102</v>
-      </c>
       <c r="G6" s="4" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B7" s="6">
         <v>2</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="4"/>
+      <c r="C7" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>107</v>
+      </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
     </row>

</xml_diff>

<commit_message>
Presentation for the converence
</commit_message>
<xml_diff>
--- a/References/Literature Review - ERASMUS Project.xlsx
+++ b/References/Literature Review - ERASMUS Project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\axelh\OneDrive\Documents\Hydroinformatics\ERASMUS_Project\References\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A9CC26A-B2DD-4FFB-9310-4577EEB88852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F90CD2CD-0AFE-42A2-B572-C475890DBB96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{33D79010-2EAD-46DA-9565-688F701BD65C}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="125">
   <si>
     <t>FOR: IRRIGATION SCHEDULING</t>
   </si>
@@ -390,9 +390,6 @@
     <t>Journal Publisher</t>
   </si>
   <si>
-    <t>FOR: LEAKAGE MODELLING</t>
-  </si>
-  <si>
     <t>Publisher</t>
   </si>
   <si>
@@ -417,13 +414,64 @@
     <t>Elsevier - Agricultural Water Management</t>
   </si>
   <si>
-    <t>Pressure and flow meter sensors.</t>
-  </si>
-  <si>
-    <t>Flow meter sensors.</t>
-  </si>
-  <si>
     <t>The zone with the most leakage was identified by analysing the result of pressure sensors. Node demands and pipe roughness were calibrated with a metaheuristic optimization algorithm. Then the probability of leakage in each sub-zone was estimated.</t>
+  </si>
+  <si>
+    <t>Locating Multiple Leaks in Water Distribution Networks Combining Physically Based and Data-Driven Models and High-Performance Computing</t>
+  </si>
+  <si>
+    <t>2023</t>
+  </si>
+  <si>
+    <t>American Society of Civil Engineers</t>
+  </si>
+  <si>
+    <t>A data-driven approach to locate multiple leaks in WDS using pressure residuals. Involving two phases, one phase to produce data sets to train classification model and perform clustering, and the other phase to estimate the location of the leaks.</t>
+  </si>
+  <si>
+    <t>- Calibrated hydraulic model.
+- Pressure sensors</t>
+  </si>
+  <si>
+    <t>- High computational demand</t>
+  </si>
+  <si>
+    <t>Leak Location Approach</t>
+  </si>
+  <si>
+    <t>Hydraulic Model Based</t>
+  </si>
+  <si>
+    <t>- Pressure sensors.
+- Flow meter sensors.</t>
+  </si>
+  <si>
+    <t>- Flow meter sensors.</t>
+  </si>
+  <si>
+    <t>Deep Learning Identifies Accurate Burst Locations in Water Distribution Networks</t>
+  </si>
+  <si>
+    <t>FOR: LEAKAGE MODELLING, LEAKAGE DETECTION, LEAKAGE LOCALIZATION</t>
+  </si>
+  <si>
+    <t>- Calibrated hydraulic model.
+- Pressure sensors.</t>
+  </si>
+  <si>
+    <t>Elsevier - Water Research</t>
+  </si>
+  <si>
+    <t>2019</t>
+  </si>
+  <si>
+    <t>A Proof-of-Concept Study for Hydraulic Model-Based Leakage Detection in Water Pipelines Using Pressure Monitoring Data</t>
+  </si>
+  <si>
+    <t>Frontiers in Water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optimization algorithm is used to predict </t>
   </si>
 </sst>
 </file>
@@ -1449,22 +1497,22 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7117D393-370F-41E6-8475-B08505AFF5F4}">
-  <dimension ref="B2:I19"/>
+  <dimension ref="B2:J19"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:F8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.77734375" style="1" customWidth="1"/>
     <col min="2" max="2" width="5.77734375" style="8" customWidth="1"/>
-    <col min="3" max="9" width="35.77734375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="5.77734375" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="1"/>
+    <col min="3" max="10" width="35.77734375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="5.77734375" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B2" s="9" t="s">
         <v>95</v>
       </c>
@@ -1472,15 +1520,15 @@
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B3" s="9" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" s="11" t="s">
         <v>1</v>
       </c>
@@ -1488,7 +1536,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>96</v>
@@ -1497,96 +1545,144 @@
         <v>3</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="H5" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="I5" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="12" t="s">
+      <c r="J5" s="12" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="2:9" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B6" s="6">
         <v>1</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="H6" s="4"/>
+      <c r="G6" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>116</v>
+      </c>
       <c r="I6" s="4"/>
-    </row>
-    <row r="7" spans="2:9" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="J6" s="4"/>
+    </row>
+    <row r="7" spans="2:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B7" s="6">
         <v>2</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>105</v>
-      </c>
       <c r="E7" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="H7" s="4"/>
+        <v>106</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="I7" s="4"/>
-    </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J7" s="4"/>
+    </row>
+    <row r="8" spans="2:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B8" s="6">
         <v>3</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C8" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" spans="2:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B9" s="6">
         <v>4</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
+      <c r="C9" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>121</v>
+      </c>
       <c r="F9" s="3"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
+      <c r="G9" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="I9" s="4"/>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J9" s="4"/>
+    </row>
+    <row r="10" spans="2:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B10" s="6">
         <v>5</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
+      <c r="C10" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="I10" s="4"/>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="6">
         <v>6</v>
       </c>
@@ -1594,11 +1690,12 @@
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
-      <c r="G11" s="4"/>
+      <c r="G11" s="3"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J11" s="4"/>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="6">
         <v>7</v>
       </c>
@@ -1606,11 +1703,12 @@
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
-      <c r="G12" s="4"/>
+      <c r="G12" s="3"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="6">
         <v>8</v>
       </c>
@@ -1618,11 +1716,12 @@
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="4"/>
+      <c r="G13" s="3"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J13" s="4"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" s="6">
         <v>9</v>
       </c>
@@ -1630,11 +1729,12 @@
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="4"/>
       <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J14" s="3"/>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" s="6">
         <v>10</v>
       </c>
@@ -1645,8 +1745,9 @@
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J15" s="3"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" s="7"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -1655,8 +1756,9 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J16" s="2"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B17" s="7"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -1665,8 +1767,9 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J17" s="2"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B18" s="7"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -1675,8 +1778,9 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="J18" s="2"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B19" s="7"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -1685,8 +1789,10 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>